<commit_message>
Change ChanceAskQuestions to a single level of missing designated "(Missing)"
</commit_message>
<xml_diff>
--- a/no_differences.xlsx
+++ b/no_differences.xlsx
@@ -5,138 +5,68 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.j.laviolette\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\OCPH\CDP\1815\1815 Epidemiology\HINTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="10260" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="10260"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1 - Table SeekCancerInfo" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2 - Table GeneralHealth" sheetId="2" r:id="rId2"/>
-    <sheet name="Table 3 - Table SeekHealthInfo" sheetId="3" r:id="rId3"/>
-    <sheet name="Table 4 - Table ChanceAskQuesti" sheetId="4" r:id="rId4"/>
-    <sheet name="Table 5 - Data Summary" sheetId="5" r:id="rId5"/>
-    <sheet name="Table 6 - Variance Estimation" sheetId="6" r:id="rId6"/>
-    <sheet name="Table 7 - Table survey   SeekHe" sheetId="7" r:id="rId7"/>
-    <sheet name="Table 8 - Table survey   Chance" sheetId="8" r:id="rId8"/>
+    <sheet name="Table 1 - Data Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 2 - Variance Estimation" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 3 - Table survey   SeekHe" sheetId="3" r:id="rId3"/>
+    <sheet name="Table 4 - Table survey   Chance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="50">
-  <si>
-    <t>A8. Have you ever looked for information about cancer from any source?</t>
-  </si>
-  <si>
-    <t>SeekCancerInfo</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="36">
+  <si>
+    <t>Data Summary</t>
+  </si>
+  <si>
+    <t>Number of Observations</t>
+  </si>
+  <si>
+    <t>Sum of Weights</t>
+  </si>
+  <si>
+    <t>Variance Estimation</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Jackknife</t>
+  </si>
+  <si>
+    <t>Replicate Weights</t>
+  </si>
+  <si>
+    <t>HINTS5_NO_DIFF</t>
+  </si>
+  <si>
+    <t>Number of Replicates</t>
+  </si>
+  <si>
+    <t>Missing Levels</t>
+  </si>
+  <si>
+    <t>Included (MISSING)</t>
+  </si>
+  <si>
+    <t>Table of survey by SeekHealthInfo</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>SeekHealthInfo</t>
   </si>
   <si>
     <t>Frequency</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Frequency Missing = 822</t>
-  </si>
-  <si>
-    <t>G1. In general, would you say your health is...</t>
-  </si>
-  <si>
-    <t>GeneralHealth</t>
-  </si>
-  <si>
-    <t>Excellent,</t>
-  </si>
-  <si>
-    <t>Very good,</t>
-  </si>
-  <si>
-    <t>Good,</t>
-  </si>
-  <si>
-    <t>Fair, or</t>
-  </si>
-  <si>
-    <t>Poor?</t>
-  </si>
-  <si>
-    <t>Frequency Missing = 175</t>
-  </si>
-  <si>
-    <t>A1. Ever looked for information about health/medical topics?</t>
-  </si>
-  <si>
-    <t>SeekHealthInfo</t>
-  </si>
-  <si>
-    <t>Frequency Missing = 164</t>
-  </si>
-  <si>
-    <t>C4a. How often...give you the chance to ask all the health-related questions you had?</t>
-  </si>
-  <si>
-    <t>ChanceAskQuestions</t>
-  </si>
-  <si>
-    <t>Always</t>
-  </si>
-  <si>
-    <t>Usually</t>
-  </si>
-  <si>
-    <t>Sometimes</t>
-  </si>
-  <si>
-    <t>Never</t>
-  </si>
-  <si>
-    <t>Frequency Missing = 2471</t>
-  </si>
-  <si>
-    <t>Data Summary</t>
-  </si>
-  <si>
-    <t>Number of Observations</t>
-  </si>
-  <si>
-    <t>Sum of Weights</t>
-  </si>
-  <si>
-    <t>Variance Estimation</t>
-  </si>
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Jackknife</t>
-  </si>
-  <si>
-    <t>Replicate Weights</t>
-  </si>
-  <si>
-    <t>HINTS5_NO_DIFF</t>
-  </si>
-  <si>
-    <t>Number of Replicates</t>
-  </si>
-  <si>
-    <t>Missing Levels</t>
-  </si>
-  <si>
-    <t>Included (MISSING)</t>
-  </si>
-  <si>
-    <t>Table of survey by SeekHealthInfo</t>
-  </si>
-  <si>
-    <t>survey</t>
   </si>
   <si>
     <t>Weighted
@@ -165,12 +95,18 @@
     <t>HINTS 5 Cycle 1</t>
   </si>
   <si>
-    <t>.</t>
+    <t>X</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
@@ -181,6 +117,24 @@
   </si>
   <si>
     <t>Table of survey by ChanceAskQuestions</t>
+  </si>
+  <si>
+    <t>ChanceAskQuestions</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>Usually</t>
+  </si>
+  <si>
+    <t>Sometimes</t>
+  </si>
+  <si>
+    <t>Never</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -190,7 +144,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,14 +284,22 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -532,6 +494,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -748,16 +716,25 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -766,12 +743,8 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1097,305 +1070,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="68.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>6404</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-  </mergeCells>
-  <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="68.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4374</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1683</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A8:B8"/>
-  </mergeCells>
-  <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="68.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>9684</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2379</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-  </mergeCells>
-  <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="92.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3">
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2658</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="3">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-  </mergeCells>
-  <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1407,22 +1084,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>25</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>12227</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>26</v>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="3">
         <v>749349378</v>
@@ -1434,19 +1111,20 @@
   </mergeCells>
   <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>Assuming No Group Differences</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1456,41 +1134,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>28</v>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>30</v>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>32</v>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>33</v>
+      <c r="A5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1499,10 +1177,13 @@
   </mergeCells>
   <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>Assuming No Group Differences</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1510,71 +1191,70 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C3" s="3">
         <v>65</v>
@@ -1591,19 +1271,19 @@
       <c r="G3" s="3">
         <v>0.14879999999999999</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="6">
         <v>2.0268000000000002</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="6">
         <v>0.4501</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="3">
         <v>2593</v>
@@ -1620,19 +1300,19 @@
       <c r="G4" s="3">
         <v>0.3765</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="6">
         <v>78.420100000000005</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="6">
         <v>1.1384000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C5" s="3">
         <v>627</v>
@@ -1649,19 +1329,19 @@
       <c r="G5" s="3">
         <v>0.37309999999999999</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="6">
         <v>19.553000000000001</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="6">
         <v>1.1282000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>46</v>
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C6" s="3">
         <v>3285</v>
@@ -1682,15 +1362,15 @@
         <v>100</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>44</v>
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C7" s="3">
         <v>10</v>
@@ -1707,19 +1387,19 @@
       <c r="G7" s="3">
         <v>4.4499999999999998E-2</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="6">
         <v>0.31009999999999999</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="6">
         <v>0.1336</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3</v>
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="3">
         <v>2786</v>
@@ -1736,19 +1416,19 @@
       <c r="G8" s="3">
         <v>0.44330000000000003</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="6">
         <v>79.083699999999993</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="6">
         <v>1.3313999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C9" s="3">
         <v>708</v>
@@ -1765,19 +1445,19 @@
       <c r="G9" s="3">
         <v>0.43630000000000002</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="6">
         <v>20.606100000000001</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="6">
         <v>1.3106</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>46</v>
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C10" s="3">
         <v>3504</v>
@@ -1798,15 +1478,15 @@
         <v>100</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>44</v>
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>89</v>
@@ -1823,19 +1503,19 @@
       <c r="G11" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="6">
         <v>1.1920999999999999</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="6">
         <v>0.2082</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>3</v>
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="3">
         <v>4305</v>
@@ -1852,19 +1532,19 @@
       <c r="G12" s="3">
         <v>0.36259999999999998</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="6">
         <v>77.691999999999993</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="6">
         <v>1.0778000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C13" s="3">
         <v>1044</v>
@@ -1881,19 +1561,19 @@
       <c r="G13" s="3">
         <v>0.36980000000000002</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="6">
         <v>21.1159</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="6">
         <v>1.0992999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>46</v>
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="3">
         <v>5438</v>
@@ -1914,15 +1594,15 @@
         <v>100</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>44</v>
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C15" s="3">
         <v>164</v>
@@ -1940,18 +1620,18 @@
         <v>0.1704</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>3</v>
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="3">
         <v>9684</v>
@@ -1969,18 +1649,18 @@
         <v>0.68530000000000002</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>4</v>
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C17" s="3">
         <v>2379</v>
@@ -1998,18 +1678,18 @@
         <v>0.68289999999999995</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>46</v>
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C18" s="3">
         <v>12227</v>
@@ -2024,13 +1704,13 @@
         <v>100</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2039,82 +1719,84 @@
   </mergeCells>
   <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>Assuming No Group Differences</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>42</v>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>44</v>
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="3">
         <v>514</v>
@@ -2131,19 +1813,19 @@
       <c r="G3" s="3">
         <v>0.38240000000000002</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="6">
         <v>18.360900000000001</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="6">
         <v>1.1563000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="3">
         <v>1765</v>
@@ -2160,19 +1842,19 @@
       <c r="G4" s="3">
         <v>0.54310000000000003</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="6">
         <v>50.140900000000002</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="6">
         <v>1.6425000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>20</v>
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="3">
         <v>725</v>
@@ -2189,19 +1871,19 @@
       <c r="G5" s="3">
         <v>0.39229999999999998</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="6">
         <v>22.321200000000001</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="6">
         <v>1.1862999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>21</v>
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="3">
         <v>245</v>
@@ -2218,19 +1900,19 @@
       <c r="G6" s="3">
         <v>0.29759999999999998</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="6">
         <v>8.3552</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="6">
         <v>0.9</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="3">
         <v>36</v>
@@ -2247,19 +1929,19 @@
       <c r="G7" s="3">
         <v>6.8500000000000005E-2</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="6">
         <v>0.82169999999999999</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="6">
         <v>0.2072</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>46</v>
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C8" s="3">
         <v>3285</v>
@@ -2280,15 +1962,15 @@
         <v>100</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>44</v>
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="3">
         <v>559</v>
@@ -2305,19 +1987,19 @@
       <c r="G9" s="3">
         <v>0.4274</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="6">
         <v>20.063800000000001</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="6">
         <v>1.2838000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C10" s="3">
         <v>1874</v>
@@ -2334,19 +2016,19 @@
       <c r="G10" s="3">
         <v>0.4259</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="6">
         <v>50.214599999999997</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="6">
         <v>1.2791999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C11" s="3">
         <v>807</v>
@@ -2363,19 +2045,19 @@
       <c r="G11" s="3">
         <v>0.39350000000000002</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="6">
         <v>23.3901</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="6">
         <v>1.1819</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="3">
         <v>228</v>
@@ -2392,19 +2074,19 @@
       <c r="G12" s="3">
         <v>0.2077</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="6">
         <v>5.3878000000000004</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="6">
         <v>0.62380000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C13" s="3">
         <v>36</v>
@@ -2421,19 +2103,19 @@
       <c r="G13" s="3">
         <v>7.3599999999999999E-2</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="6">
         <v>0.94369999999999998</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="6">
         <v>0.221</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>46</v>
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="3">
         <v>3504</v>
@@ -2454,15 +2136,15 @@
         <v>100</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>44</v>
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C15" s="3">
         <v>1398</v>
@@ -2479,19 +2161,19 @@
       <c r="G15" s="3">
         <v>0.3821</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="6">
         <v>28.020099999999999</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="6">
         <v>1.1359999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>19</v>
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C16" s="3">
         <v>2611</v>
@@ -2508,19 +2190,19 @@
       <c r="G16" s="3">
         <v>0.41299999999999998</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="6">
         <v>45.211199999999998</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="6">
         <v>1.2279</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>20</v>
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C17" s="3">
         <v>1126</v>
@@ -2537,19 +2219,19 @@
       <c r="G17" s="3">
         <v>0.36120000000000002</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="6">
         <v>20.707899999999999</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="6">
         <v>1.0738000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>21</v>
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C18" s="3">
         <v>260</v>
@@ -2566,19 +2248,19 @@
       <c r="G18" s="3">
         <v>0.2132</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="6">
         <v>5.4280999999999997</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="6">
         <v>0.63390000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>22</v>
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C19" s="3">
         <v>43</v>
@@ -2595,19 +2277,19 @@
       <c r="G19" s="3">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="6">
         <v>0.63260000000000005</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="6">
         <v>0.12180000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>46</v>
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C20" s="3">
         <v>5438</v>
@@ -2628,15 +2310,15 @@
         <v>100</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>44</v>
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C21" s="3">
         <v>2471</v>
@@ -2654,18 +2336,18 @@
         <v>0.68910000000000005</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>19</v>
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C22" s="3">
         <v>6250</v>
@@ -2683,18 +2365,18 @@
         <v>0.8044</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>20</v>
+      <c r="A23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C23" s="3">
         <v>2658</v>
@@ -2712,18 +2394,18 @@
         <v>0.66269999999999996</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>21</v>
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C24" s="3">
         <v>733</v>
@@ -2741,18 +2423,18 @@
         <v>0.4209</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>22</v>
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C25" s="3">
         <v>115</v>
@@ -2770,18 +2452,18 @@
         <v>0.1086</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>46</v>
+      <c r="A26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C26" s="3">
         <v>12227</v>
@@ -2796,13 +2478,13 @@
         <v>100</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2811,5 +2493,8 @@
   </mergeCells>
   <pageMargins left="0.08" right="0.08" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="100" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>Assuming No Group Differences</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>